<commit_message>
upd welcome and gitignore
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngiordano\OneDrive - Kansas State University\Desktop\KSU-WHEAT-APP-main-2.0\IDataField-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9B017C-49C2-42BD-AFC9-DAFEE2A1775B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9945D-90A6-4DCD-8104-AB748DE1690C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9888" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LABELS_INPUT" sheetId="1" r:id="rId1"/>
-    <sheet name="Trials And Locations" sheetId="2" r:id="rId2"/>
-    <sheet name="Activities" sheetId="3" r:id="rId3"/>
-    <sheet name="Phenology" sheetId="4" r:id="rId4"/>
-    <sheet name="Plant_Traits" sheetId="7" r:id="rId5"/>
-    <sheet name="Columns" sheetId="5" r:id="rId6"/>
-    <sheet name="Columns names" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="Trials And Locations" sheetId="2" r:id="rId3"/>
+    <sheet name="Activities" sheetId="3" r:id="rId4"/>
+    <sheet name="Phenology" sheetId="4" r:id="rId5"/>
+    <sheet name="Plant_Traits" sheetId="7" r:id="rId6"/>
+    <sheet name="Columns" sheetId="5" r:id="rId7"/>
+    <sheet name="Column Description" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LABELS_INPUT!$A$1:$I$310</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Trials And Locations'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Trials And Locations'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="285">
   <si>
     <t>YEAR</t>
   </si>
@@ -878,6 +879,18 @@
   </si>
   <si>
     <t>F11.4</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grain yield </t>
+  </si>
+  <si>
+    <t>Stand count spring</t>
+  </si>
+  <si>
+    <t>SCS</t>
   </si>
 </sst>
 </file>
@@ -2421,9 +2434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I197" sqref="I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13028,6 +13041,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E757A881-E26C-4178-B684-57531D1649A8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
@@ -13841,12 +13866,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF72BDF-E972-4DFC-8739-BD42FEEE886B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13895,17 +13920,25 @@
         <v>220</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B6" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF5B107-C584-4390-A6DE-85AC76E074C1}">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14003,12 +14036,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CF0237-5540-47AA-B2E5-9CB697CBA0FE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14053,7 +14086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312657E8-3DEA-4EE1-BA23-8DC32180507F}">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -14218,18 +14251,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CCF87D-BB28-48CE-9ACE-15B308A318FF}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -14238,6 +14271,14 @@
       </c>
       <c r="B1" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -14246,6 +14287,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004985193A87153942845D241572937CE5" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41d807227133e919f3755c54a0ed2601">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff" xmlns:ns4="f703b2de-b014-43d1-91b4-4178b52ec481" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="28768a436f2ded89381638814bc7efce" ns3:_="" ns4:_="">
     <xsd:import namespace="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff"/>
@@ -14486,24 +14544,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80E2AB2F-6E1F-424C-8E97-B29CFF39A56D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309818C2-C029-41E7-90B5-C5C7A9CD1F23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3154782E-A8FB-4B5D-908B-67EB26D31F14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14520,22 +14579,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309818C2-C029-41E7-90B5-C5C7A9CD1F23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80E2AB2F-6E1F-424C-8E97-B29CFF39A56D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>